<commit_message>
gui working much better
</commit_message>
<xml_diff>
--- a/CHAT3-4.xlsx
+++ b/CHAT3-4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speard\Documents\Moorings\Projects\Chatham Sound\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{48AE4198-38DE-49BA-A1E1-80A785654ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1822BB-DD4E-468D-8AC5-23DF29E091AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12754" windowHeight="4954" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>5/16" Amsteel II+</t>
   </si>
   <si>
-    <t xml:space="preserve">estimated Amsteel II+ stretch   </t>
-  </si>
-  <si>
     <t>SM2M+ in Frame</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>SeapHox in Frame</t>
+  </si>
+  <si>
+    <t>Anchor</t>
   </si>
 </sst>
 </file>
@@ -1302,32 +1302,32 @@
   </sheetPr>
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.15234375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.69140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="10.69140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.15234375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="13.84375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="10.69140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="10.53515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.15234375" style="7"/>
+    <col min="1" max="1" width="28.109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>160</v>
       </c>
@@ -1335,10 +1335,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
     </row>
-    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>4</v>
@@ -1359,7 +1359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="11" customFormat="1" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17" t="s">
         <v>8</v>
@@ -1380,7 +1380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.6" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="21"/>
       <c r="C6" s="22"/>
@@ -1390,7 +1390,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>23</v>
       </c>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="H7" s="93"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="G8" s="33"/>
       <c r="H8" s="93"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>0</v>
       </c>
@@ -1457,9 +1457,9 @@
       <c r="G9" s="33"/>
       <c r="H9" s="93"/>
     </row>
-    <row r="10" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="35">
         <f>4.4+2.3+8.63</f>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="H10" s="94"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="G11" s="40"/>
       <c r="H11" s="93"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>21</v>
       </c>
@@ -1526,7 +1526,7 @@
       <c r="G12" s="29"/>
       <c r="H12" s="93"/>
     </row>
-    <row r="13" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>20</v>
       </c>
@@ -1546,9 +1546,9 @@
       <c r="G13" s="44"/>
       <c r="H13" s="95"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="79" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="80">
         <f>0.031*D14</f>
@@ -1571,7 +1571,7 @@
       <c r="G14" s="48"/>
       <c r="H14" s="93"/>
     </row>
-    <row r="15" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>20</v>
       </c>
@@ -1591,7 +1591,7 @@
       <c r="G15" s="44"/>
       <c r="H15" s="95"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>0</v>
       </c>
@@ -1610,9 +1610,9 @@
       <c r="G16" s="40"/>
       <c r="H16" s="93"/>
     </row>
-    <row r="17" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="35">
         <f>208+13</f>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="H17" s="94"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1658,7 @@
       <c r="G18" s="40"/>
       <c r="H18" s="93"/>
     </row>
-    <row r="19" spans="1:10" s="86" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="86" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="82" t="s">
         <v>0</v>
       </c>
@@ -1677,9 +1677,9 @@
       <c r="G19" s="85"/>
       <c r="H19" s="96"/>
     </row>
-    <row r="20" spans="1:10" s="90" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" s="90" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="88">
         <f>13+13.5</f>
@@ -1707,7 +1707,7 @@
       <c r="H20" s="97"/>
       <c r="I20" s="91"/>
     </row>
-    <row r="21" spans="1:10" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="92" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1726,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="98"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>0</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="G22" s="40"/>
       <c r="H22" s="93"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>18</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="G23" s="40"/>
       <c r="H23" s="93"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="G24" s="40"/>
       <c r="H24" s="93"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>21</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="G25" s="29"/>
       <c r="H25" s="93"/>
     </row>
-    <row r="26" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>20</v>
       </c>
@@ -1824,7 +1824,7 @@
       <c r="G26" s="44"/>
       <c r="H26" s="95"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>24</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="G27" s="54"/>
       <c r="H27" s="93"/>
     </row>
-    <row r="28" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>20</v>
       </c>
@@ -1867,7 +1867,7 @@
       <c r="G28" s="44"/>
       <c r="H28" s="95"/>
     </row>
-    <row r="29" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>0</v>
       </c>
@@ -1886,9 +1886,9 @@
       <c r="G29" s="40"/>
       <c r="H29" s="99"/>
     </row>
-    <row r="30" spans="1:10" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>76</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="H30" s="98"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>0</v>
       </c>
@@ -1926,9 +1926,9 @@
       <c r="G31" s="40"/>
       <c r="H31" s="93"/>
     </row>
-    <row r="32" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="35">
         <f>13+13.5</f>
@@ -1954,7 +1954,7 @@
       <c r="I32" s="58"/>
       <c r="J32" s="57"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="30" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="G33" s="40"/>
       <c r="H33" s="93"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="30" t="s">
         <v>0</v>
       </c>
@@ -1992,9 +1992,9 @@
       <c r="G34" s="40"/>
       <c r="H34" s="93"/>
     </row>
-    <row r="35" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="35">
         <f>13+13.5</f>
@@ -2020,7 +2020,7 @@
       <c r="I35" s="58"/>
       <c r="J35" s="57"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="30" t="s">
         <v>0</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="G36" s="40"/>
       <c r="H36" s="93"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>0</v>
       </c>
@@ -2058,9 +2058,9 @@
       <c r="G37" s="40"/>
       <c r="H37" s="93"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="35">
         <f>4.4+2.3+8.63</f>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="H38" s="93"/>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30" t="s">
         <v>0</v>
       </c>
@@ -2103,7 +2103,7 @@
       <c r="G39" s="40"/>
       <c r="H39" s="93"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="30" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="G40" s="40"/>
       <c r="H40" s="93"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
         <v>18</v>
       </c>
@@ -2141,7 +2141,7 @@
       <c r="G41" s="40"/>
       <c r="H41" s="93"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="30" t="s">
         <v>0</v>
       </c>
@@ -2160,7 +2160,7 @@
       <c r="G42" s="40"/>
       <c r="H42" s="93"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>21</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="G43" s="29"/>
       <c r="H43" s="93"/>
     </row>
-    <row r="44" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
         <v>20</v>
       </c>
@@ -2201,7 +2201,7 @@
       <c r="G44" s="44"/>
       <c r="H44" s="95"/>
     </row>
-    <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
         <v>24</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="G45" s="61"/>
       <c r="H45" s="93"/>
     </row>
-    <row r="46" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
         <v>20</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="G46" s="44"/>
       <c r="H46" s="95"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>0</v>
       </c>
@@ -2263,9 +2263,9 @@
       <c r="G47" s="40"/>
       <c r="H47" s="93"/>
     </row>
-    <row r="48" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B48" s="35">
         <f>362+86+4</f>
@@ -2291,7 +2291,7 @@
       <c r="I48" s="58"/>
       <c r="J48" s="58"/>
     </row>
-    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2310,7 @@
       <c r="G49" s="40"/>
       <c r="H49" s="93"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>0</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="G50" s="40"/>
       <c r="H50" s="93"/>
     </row>
-    <row r="51" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50" t="s">
         <v>1</v>
       </c>
@@ -2347,7 +2347,7 @@
       <c r="G51" s="40"/>
       <c r="H51" s="101"/>
     </row>
-    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2366,7 @@
       <c r="G52" s="65"/>
       <c r="H52" s="93"/>
     </row>
-    <row r="53" spans="1:8" s="68" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" s="68" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="66" t="s">
         <v>15</v>
       </c>
@@ -2386,7 +2386,7 @@
       <c r="G53" s="67"/>
       <c r="H53" s="102"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
         <v>14</v>
       </c>
@@ -2407,7 +2407,7 @@
       <c r="G54" s="38"/>
       <c r="H54" s="93"/>
     </row>
-    <row r="55" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="30" t="s">
         <v>16</v>
       </c>
@@ -2424,7 +2424,7 @@
       <c r="G55" s="40"/>
       <c r="H55" s="95"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="70" t="s">
         <v>17</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="G56" s="48"/>
       <c r="H56" s="93"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="30" t="s">
         <v>2</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="G57" s="40"/>
       <c r="H57" s="93"/>
     </row>
-    <row r="58" spans="1:8" ht="14.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="71" t="s">
         <v>3</v>
       </c>
@@ -2481,16 +2481,16 @@
       <c r="G58" s="74"/>
       <c r="H58" s="93"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="75" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B59" s="76">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H59" s="93"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="77"/>
       <c r="C60" s="78"/>
     </row>
@@ -2510,9 +2510,9 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>360</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>720</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>3*360</f>
         <v>1080</v>
@@ -2560,7 +2560,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>